<commit_message>
Committed changes for latest updates
</commit_message>
<xml_diff>
--- a/Katalon End to End WebApp Project using virtual Devices(BrowserStack)/Data Files/dataFile.xlsx
+++ b/Katalon End to End WebApp Project using virtual Devices(BrowserStack)/Data Files/dataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>User Name</t>
   </si>
@@ -277,6 +277,42 @@
   </si>
   <si>
     <t>Test18042025@438</t>
+  </si>
+  <si>
+    <t>Test18042025@309.com</t>
+  </si>
+  <si>
+    <t>Test18042025@309</t>
+  </si>
+  <si>
+    <t>Test18042025@207.com</t>
+  </si>
+  <si>
+    <t>Test18042025@207</t>
+  </si>
+  <si>
+    <t>Test18042025@350.com</t>
+  </si>
+  <si>
+    <t>Test18042025@350</t>
+  </si>
+  <si>
+    <t>Test18042025@538.com</t>
+  </si>
+  <si>
+    <t>Test18042025@538</t>
+  </si>
+  <si>
+    <t>Test18042025@496.com</t>
+  </si>
+  <si>
+    <t>Test18042025@496</t>
+  </si>
+  <si>
+    <t>Test18042025@289.com</t>
+  </si>
+  <si>
+    <t>Test18042025@289</t>
   </si>
 </sst>
 </file>
@@ -636,10 +672,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C2" s="3"/>
     </row>

</xml_diff>

<commit_message>
Katalon API Project commit
</commit_message>
<xml_diff>
--- a/Katalon End to End WebApp Project using virtual Devices(BrowserStack)/Data Files/dataFile.xlsx
+++ b/Katalon End to End WebApp Project using virtual Devices(BrowserStack)/Data Files/dataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>User Name</t>
   </si>
@@ -313,6 +313,24 @@
   </si>
   <si>
     <t>Test18042025@289</t>
+  </si>
+  <si>
+    <t>Test18042025@460.com</t>
+  </si>
+  <si>
+    <t>Test18042025@460</t>
+  </si>
+  <si>
+    <t>Test18042025@196.com</t>
+  </si>
+  <si>
+    <t>Test18042025@196</t>
+  </si>
+  <si>
+    <t>Test18042025@821.com</t>
+  </si>
+  <si>
+    <t>Test18042025@821</t>
   </si>
 </sst>
 </file>
@@ -672,10 +690,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C2" s="3"/>
     </row>

</xml_diff>